<commit_message>
add saled count/ all the house count in the code
Signed-off-by: Richard Xiong <yong.xiong@nxp.com>
</commit_message>
<xml_diff>
--- a/projects/python3/house_price/dist/house.xlsx
+++ b/projects/python3/house_price/dist/house.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,6 +570,16 @@
           <t>1504</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -591,6 +601,12 @@
         <is>
           <t>1404</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -890,7 +906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -993,6 +1009,16 @@
           <t>2404</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1014,6 +1040,12 @@
         <is>
           <t>2304</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="6">
@@ -1501,7 +1533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1604,6 +1636,16 @@
           <t>2404</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1625,6 +1667,12 @@
         <is>
           <t>2304</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="6">
@@ -2112,7 +2160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2215,6 +2263,16 @@
           <t>2404</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2236,6 +2294,12 @@
         <is>
           <t>2304</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -2733,7 +2797,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2836,6 +2900,16 @@
           <t>1204</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -2857,6 +2931,12 @@
         <is>
           <t>1104</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -3085,7 +3165,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3188,6 +3268,16 @@
           <t>1504</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -3209,6 +3299,12 @@
         <is>
           <t>1404</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -3508,7 +3604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3611,6 +3707,16 @@
           <t>2404</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -3632,6 +3738,12 @@
         <is>
           <t>2304</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -4129,7 +4241,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4232,6 +4344,16 @@
           <t>1504</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -4253,6 +4375,12 @@
         <is>
           <t>1404</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -4552,7 +4680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4655,6 +4783,16 @@
           <t>1204</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -4676,6 +4814,12 @@
         <is>
           <t>1104</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -4899,7 +5043,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5002,6 +5146,16 @@
           <t>1504</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -5023,6 +5177,12 @@
         <is>
           <t>1404</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -5322,7 +5482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5425,6 +5585,16 @@
           <t>1404</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -5446,6 +5616,12 @@
         <is>
           <t>1304</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="6">
@@ -5723,7 +5899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5826,6 +6002,16 @@
           <t>1404</t>
         </is>
       </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>未售</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>总量</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -5847,6 +6033,12 @@
         <is>
           <t>1304</t>
         </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="6">

</xml_diff>